<commit_message>
feat: update BlessUI language
更新祝福UI多语言
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Language_多语言.xlsx
+++ b/nevergiveup/Excel/Language_多语言.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8835A03F-8178-4EBC-9B2B-6D63D2AA328C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCD7C03-DE47-4FE7-950A-351339EA098B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="2594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="2600">
   <si>
     <t>Int</t>
   </si>
@@ -13457,6 +13457,30 @@
   </si>
   <si>
     <t>Deep Cavern - Hard</t>
+  </si>
+  <si>
+    <t>Bless_UI_1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>祝福</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>*龙娘祝福来自于 Dragonverse 主世界通过“蓝色飞贼”抓取的龙娘</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blessing</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>*The Modragon's blessing comes from the Modragon captured by the "Blue Snitch" in the DragonverseNeo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bless_UI_2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -14422,10 +14446,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ1452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A440" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C142" sqref="C142"/>
+      <selection pane="bottomLeft" activeCell="E458" sqref="E458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -23485,23 +23509,39 @@
       <c r="F457" s="4"/>
     </row>
     <row r="458" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A458" s="4"/>
-      <c r="B458" s="2"/>
-      <c r="C458" s="29"/>
-      <c r="D458" s="5"/>
+      <c r="A458" s="1">
+        <v>20453</v>
+      </c>
+      <c r="B458" s="2" t="s">
+        <v>2594</v>
+      </c>
+      <c r="C458" s="27" t="s">
+        <v>2597</v>
+      </c>
+      <c r="D458" s="5" t="s">
+        <v>2595</v>
+      </c>
       <c r="E458" s="2"/>
       <c r="F458" s="4"/>
     </row>
-    <row r="459" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A459" s="4"/>
-      <c r="B459" s="2"/>
-      <c r="C459" s="29"/>
-      <c r="D459" s="5"/>
+    <row r="459" spans="1:6" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A459" s="1">
+        <v>20454</v>
+      </c>
+      <c r="B459" s="2" t="s">
+        <v>2599</v>
+      </c>
+      <c r="C459" s="27" t="s">
+        <v>2598</v>
+      </c>
+      <c r="D459" s="5" t="s">
+        <v>2596</v>
+      </c>
       <c r="E459" s="2"/>
       <c r="F459" s="4"/>
     </row>
     <row r="460" spans="1:6" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A460" s="4"/>
+      <c r="A460" s="1"/>
       <c r="B460" s="2"/>
       <c r="C460" s="29"/>
       <c r="D460" s="5"/>

</xml_diff>

<commit_message>
feat: update Asset and UI
去除npc名字 调整UI
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Language_多语言.xlsx
+++ b/nevergiveup/Excel/Language_多语言.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA2AB25-3217-45B7-80FE-BEAAF176DE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2012FA6-3315-49B2-91D9-148A027A497B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3332" uniqueCount="3047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3332" uniqueCount="3049">
   <si>
     <t>Int</t>
   </si>
@@ -14445,10 +14445,6 @@
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
   <si>
-    <t>Attack Range</t>
-    <phoneticPr fontId="22" type="noConversion"/>
-  </si>
-  <si>
     <t>召唤·光I</t>
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
@@ -14533,10 +14529,6 @@
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
   <si>
-    <t>Apex Magical</t>
-    <phoneticPr fontId="22" type="noConversion"/>
-  </si>
-  <si>
     <t>TalentBuff_Name_2002</t>
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
@@ -14581,11 +14573,27 @@
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
   <si>
-    <t>Attack Speed</t>
+    <t>Decel+</t>
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
   <si>
-    <t>Decel+</t>
+    <t>Atk Speed</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>Physical</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>Magical</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dura</t>
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
 </sst>
@@ -15267,8 +15275,8 @@
   <dimension ref="A1:AMJ1434"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C381" sqref="C381"/>
+      <pane ySplit="3" topLeftCell="A647" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D682" sqref="D682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -15529,10 +15537,10 @@
         <v>34</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>3040</v>
+        <v>3038</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>3039</v>
+        <v>3037</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -16538,10 +16546,10 @@
         <v>20053</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>3027</v>
+        <v>3026</v>
       </c>
       <c r="C58" s="56" t="s">
-        <v>3030</v>
+        <v>3029</v>
       </c>
       <c r="D58" s="17" t="s">
         <v>165</v>
@@ -22247,7 +22255,7 @@
         <v>936</v>
       </c>
       <c r="C326" s="7" t="s">
-        <v>3044</v>
+        <v>3042</v>
       </c>
       <c r="D326" s="7" t="s">
         <v>938</v>
@@ -24012,7 +24020,7 @@
         <v>20433</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>3026</v>
+        <v>3025</v>
       </c>
       <c r="C438" s="10" t="s">
         <v>1222</v>
@@ -24876,7 +24884,7 @@
         <v>1371</v>
       </c>
       <c r="D491" s="22" t="s">
-        <v>3014</v>
+        <v>3013</v>
       </c>
       <c r="F491" s="9"/>
     </row>
@@ -24921,7 +24929,7 @@
         <v>1376</v>
       </c>
       <c r="D494" s="22" t="s">
-        <v>3013</v>
+        <v>3012</v>
       </c>
       <c r="F494" s="9"/>
     </row>
@@ -25146,7 +25154,7 @@
         <v>1405</v>
       </c>
       <c r="D509" s="55" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="F509" s="9"/>
     </row>
@@ -25611,7 +25619,7 @@
         <v>1464</v>
       </c>
       <c r="D539" s="37" t="s">
-        <v>3012</v>
+        <v>3011</v>
       </c>
       <c r="E539" s="6"/>
       <c r="F539" s="9"/>
@@ -25627,7 +25635,7 @@
         <v>1465</v>
       </c>
       <c r="D540" s="37" t="s">
-        <v>3015</v>
+        <v>3014</v>
       </c>
       <c r="E540" s="6"/>
       <c r="F540" s="9"/>
@@ -25643,7 +25651,7 @@
         <v>1466</v>
       </c>
       <c r="D541" s="10" t="s">
-        <v>3016</v>
+        <v>3015</v>
       </c>
       <c r="E541" s="6"/>
       <c r="F541" s="9"/>
@@ -25659,7 +25667,7 @@
         <v>1467</v>
       </c>
       <c r="D542" s="10" t="s">
-        <v>3017</v>
+        <v>3016</v>
       </c>
       <c r="E542" s="6"/>
       <c r="F542" s="9"/>
@@ -25675,7 +25683,7 @@
         <v>1468</v>
       </c>
       <c r="D543" s="10" t="s">
-        <v>3018</v>
+        <v>3017</v>
       </c>
       <c r="E543" s="6"/>
       <c r="F543" s="9"/>
@@ -25691,7 +25699,7 @@
         <v>1469</v>
       </c>
       <c r="D544" s="10" t="s">
-        <v>3019</v>
+        <v>3018</v>
       </c>
       <c r="E544" s="6"/>
       <c r="F544" s="9"/>
@@ -27423,13 +27431,13 @@
         <v>20654</v>
       </c>
       <c r="B659" s="6" t="s">
-        <v>3032</v>
+        <v>3031</v>
       </c>
       <c r="C659" s="54" t="s">
-        <v>3010</v>
+        <v>3045</v>
       </c>
       <c r="D659" s="37" t="s">
-        <v>3020</v>
+        <v>3019</v>
       </c>
       <c r="E659" s="26"/>
     </row>
@@ -27438,13 +27446,13 @@
         <v>20655</v>
       </c>
       <c r="B660" s="6" t="s">
-        <v>3034</v>
+        <v>3032</v>
       </c>
       <c r="C660" s="54" t="s">
-        <v>3033</v>
+        <v>3046</v>
       </c>
       <c r="D660" s="37" t="s">
-        <v>3021</v>
+        <v>3020</v>
       </c>
       <c r="E660" s="26"/>
     </row>
@@ -27453,13 +27461,13 @@
         <v>20656</v>
       </c>
       <c r="B661" s="6" t="s">
-        <v>3035</v>
+        <v>3033</v>
       </c>
       <c r="C661" s="54" t="s">
-        <v>3011</v>
+        <v>3047</v>
       </c>
       <c r="D661" s="37" t="s">
-        <v>3022</v>
+        <v>3021</v>
       </c>
       <c r="E661" s="26"/>
     </row>
@@ -27468,13 +27476,13 @@
         <v>20657</v>
       </c>
       <c r="B662" s="6" t="s">
-        <v>3036</v>
+        <v>3034</v>
       </c>
       <c r="C662" s="7" t="s">
-        <v>3046</v>
+        <v>3043</v>
       </c>
       <c r="D662" s="38" t="s">
-        <v>3023</v>
+        <v>3022</v>
       </c>
       <c r="E662" s="26"/>
     </row>
@@ -27483,13 +27491,13 @@
         <v>20658</v>
       </c>
       <c r="B663" s="6" t="s">
-        <v>3037</v>
-      </c>
-      <c r="C663" s="28" t="s">
-        <v>1159</v>
+        <v>3035</v>
+      </c>
+      <c r="C663" s="54" t="s">
+        <v>3048</v>
       </c>
       <c r="D663" s="37" t="s">
-        <v>3024</v>
+        <v>3023</v>
       </c>
       <c r="E663" s="26"/>
     </row>
@@ -27498,13 +27506,13 @@
         <v>20659</v>
       </c>
       <c r="B664" s="6" t="s">
-        <v>3038</v>
+        <v>3036</v>
       </c>
       <c r="C664" s="7" t="s">
-        <v>3045</v>
+        <v>3044</v>
       </c>
       <c r="D664" s="37" t="s">
-        <v>3025</v>
+        <v>3024</v>
       </c>
       <c r="E664" s="26"/>
     </row>
@@ -27513,13 +27521,13 @@
         <v>20660</v>
       </c>
       <c r="B665" s="6" t="s">
+        <v>3027</v>
+      </c>
+      <c r="C665" s="57" t="s">
+        <v>3030</v>
+      </c>
+      <c r="D665" s="7" t="s">
         <v>3028</v>
-      </c>
-      <c r="C665" s="57" t="s">
-        <v>3031</v>
-      </c>
-      <c r="D665" s="7" t="s">
-        <v>3029</v>
       </c>
       <c r="E665" s="26"/>
     </row>
@@ -27528,13 +27536,13 @@
         <v>20661</v>
       </c>
       <c r="B666" s="6" t="s">
+        <v>3039</v>
+      </c>
+      <c r="C666" s="57" t="s">
+        <v>3040</v>
+      </c>
+      <c r="D666" s="7" t="s">
         <v>3041</v>
-      </c>
-      <c r="C666" s="57" t="s">
-        <v>3042</v>
-      </c>
-      <c r="D666" s="7" t="s">
-        <v>3043</v>
       </c>
       <c r="E666" s="26"/>
     </row>

</xml_diff>

<commit_message>
feat: update stage reward
更新完美通关塔奖励
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Language_多语言.xlsx
+++ b/nevergiveup/Excel/Language_多语言.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\editor_v0.40.0.2.20241015185135\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\nevergiveup\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CEE9FD-0A5F-4D66-A355-A736EEDB919A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D5D858-F789-4873-AF9A-7AD03D5CB08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3377" uniqueCount="3204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="3207">
   <si>
     <t>Int</t>
   </si>
@@ -15132,6 +15132,18 @@
   </si>
   <si>
     <t>完美·世界1</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否确认以500金币的价格将塔回收给商店</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Text_TowerReturn</t>
+    <phoneticPr fontId="17" type="noConversion"/>
+  </si>
+  <si>
+    <t>Are you sure you want to recycle the tower back to the shop for 500 gold?</t>
     <phoneticPr fontId="17" type="noConversion"/>
   </si>
 </sst>
@@ -15748,8 +15760,8 @@
   <dimension ref="A1:AMJ692"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A504" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C525" sqref="C525"/>
+      <pane ySplit="3" topLeftCell="A656" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E682" sqref="E682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -28240,11 +28252,19 @@
       </c>
       <c r="E681" s="26"/>
     </row>
-    <row r="682" spans="1:5" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A682" s="9"/>
-      <c r="B682" s="6"/>
-      <c r="C682" s="11"/>
-      <c r="D682" s="14"/>
+    <row r="682" spans="1:5" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A682" s="12">
+        <v>20677</v>
+      </c>
+      <c r="B682" s="6" t="s">
+        <v>3205</v>
+      </c>
+      <c r="C682" s="11" t="s">
+        <v>3206</v>
+      </c>
+      <c r="D682" s="14" t="s">
+        <v>3204</v>
+      </c>
       <c r="E682" s="26"/>
     </row>
     <row r="683" spans="1:5" s="5" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
game ui for s9 beta
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Language_多语言.xlsx
+++ b/nevergiveup/Excel/Language_多语言.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17600" tabRatio="500"/>
+    <workbookView windowHeight="17150" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4536,19 +4536,19 @@
     <t>Task_taskName_55</t>
   </si>
   <si>
-    <t>Finish 2 game</t>
-  </si>
-  <si>
-    <t>完成2局游戏</t>
+    <t>Finish 5 game</t>
+  </si>
+  <si>
+    <t>完成5局游戏</t>
   </si>
   <si>
     <t>Task_taskName_56</t>
   </si>
   <si>
-    <t>Finish 1 game with Perfection</t>
-  </si>
-  <si>
-    <t>完成1局完美通关</t>
+    <t>Finish 10 game with Perfection</t>
+  </si>
+  <si>
+    <t>完成10局完美通关</t>
   </si>
   <si>
     <t>Task_taskName_57</t>
@@ -5190,10 +5190,10 @@
     <t>Task_taskinfo_73</t>
   </si>
   <si>
-    <t>Unlocked 1 Tower Today</t>
-  </si>
-  <si>
-    <t>今日解锁一个塔</t>
+    <t>Unlocked 2 Tower Today</t>
+  </si>
+  <si>
+    <t>今日解锁2个塔</t>
   </si>
   <si>
     <t>Return_text_1</t>
@@ -14783,7 +14783,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="35">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -14803,11 +14803,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
     <font>
@@ -15345,28 +15340,31 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -15375,121 +15373,118 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -15525,8 +15520,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -15534,52 +15532,49 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -15588,37 +15583,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -15945,9 +15940,9 @@
   <dimension ref="A1:L717"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A693" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A573" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D720" sqref="D720"/>
+      <selection pane="bottomLeft" activeCell="D620" sqref="D620"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.5"/>

</xml_diff>

<commit_message>
fix: td task solvTime config
</commit_message>
<xml_diff>
--- a/nevergiveup/Excel/Language_多语言.xlsx
+++ b/nevergiveup/Excel/Language_多语言.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18360" tabRatio="500"/>
+    <workbookView windowHeight="18375" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4536,19 +4536,19 @@
     <t>Task_taskName_55</t>
   </si>
   <si>
-    <t>Finish 5 game</t>
-  </si>
-  <si>
-    <t>完成5局游戏</t>
+    <t>Finish 10 game</t>
+  </si>
+  <si>
+    <t>完成10局游戏</t>
   </si>
   <si>
     <t>Task_taskName_56</t>
   </si>
   <si>
-    <t>Finish 10 game with Perfection</t>
-  </si>
-  <si>
-    <t>完成10局完美通关</t>
+    <t>Finish 2 game with Perfection</t>
+  </si>
+  <si>
+    <t>完成2局完美通关</t>
   </si>
   <si>
     <t>Task_taskName_57</t>
@@ -5190,10 +5190,10 @@
     <t>Task_taskinfo_73</t>
   </si>
   <si>
-    <t>Unlocked 2 Tower Today</t>
-  </si>
-  <si>
-    <t>今日解锁2个塔</t>
+    <t>Unlocked 1 Tower Today</t>
+  </si>
+  <si>
+    <t>今日解锁1个塔</t>
   </si>
   <si>
     <t>Return_text_1</t>
@@ -15958,9 +15958,9 @@
   <dimension ref="A1:L719"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A708" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A557" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C729" sqref="C729"/>
+      <selection pane="bottomLeft" activeCell="D622" sqref="D622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="16.5"/>

</xml_diff>